<commit_message>
change column1 title to #
</commit_message>
<xml_diff>
--- a/Data_GamesCompanies/Data_2209.xlsx
+++ b/Data_GamesCompanies/Data_2209.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="533">
   <si>
-    <t>Unnamed: 0</t>
+    <t>#</t>
   </si>
   <si>
     <t>Unified App</t>
@@ -1631,7 +1631,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1695,19 +1695,19 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2054,7 +2054,7 @@
     <col min="25" max="25" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="30.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="32.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>112</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>118</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>128</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>134</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>145</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>151</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>157</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>162</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>168</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="4">
         <v>25</v>
       </c>

</xml_diff>